<commit_message>
Monthly defects based on priorities of the defect
Get monthly count of defect differentiated as total defects per month
and total p1, p2,p3 defect
</commit_message>
<xml_diff>
--- a/examples/Defect - Copy.xlsx
+++ b/examples/Defect - Copy.xlsx
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="I7" sqref="I7:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +389,7 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -411,7 +411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -422,7 +422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>11</v>
       </c>
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>15</v>
       </c>
@@ -444,7 +444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>13</v>
       </c>
@@ -465,8 +465,17 @@
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I7" s="1">
+        <v>41</v>
+      </c>
+      <c r="J7" s="2">
+        <v>42005</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>14</v>
       </c>
@@ -476,8 +485,17 @@
       <c r="C8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>42</v>
+      </c>
+      <c r="J8" s="2">
+        <v>42007</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>16</v>
       </c>
@@ -487,8 +505,17 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <v>43</v>
+      </c>
+      <c r="J9" s="2">
+        <v>42005</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>17</v>
       </c>
@@ -498,8 +525,17 @@
       <c r="C10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>44</v>
+      </c>
+      <c r="J10" s="2">
+        <v>42007</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -509,8 +545,17 @@
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <v>45</v>
+      </c>
+      <c r="J11" s="2">
+        <v>42005</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -520,8 +565,17 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <v>46</v>
+      </c>
+      <c r="J12" s="2">
+        <v>42007</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -532,7 +586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>20</v>
       </c>
@@ -543,7 +597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -554,7 +608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
defect data in a dictionary
</commit_message>
<xml_diff>
--- a/examples/Defect - Copy.xlsx
+++ b/examples/Defect - Copy.xlsx
@@ -16,6 +16,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$47</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -452,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D47"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,6 +1164,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D47"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>